<commit_message>
Create gitignore. Plan and set goals for the first week
</commit_message>
<xml_diff>
--- a/doc/time_management.xlsx
+++ b/doc/time_management.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25726"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antti\Documents\Courses\BDA\Bayes_project_2022\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D93B1D2-3C88-4387-8DD9-385716DADABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,12 +24,216 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Viikko</t>
+  </si>
+  <si>
+    <t>Amanda</t>
+  </si>
+  <si>
+    <t>Anni</t>
+  </si>
+  <si>
+    <t>Antti</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>44</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (31.10.-6.11.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">45 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(7.-13.11.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">46 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(14.-20.11.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">47 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(21.-27.11.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">48 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(28.11.-4.12.)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Project DL</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 2.12.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Bayes Assignments 9</t>
+  </si>
+  <si>
+    <t>Bayes Assignmnets 8</t>
+  </si>
+  <si>
+    <t>goal</t>
+  </si>
+  <si>
+    <t>Planning the project: Find data, project plan, project schedule</t>
+  </si>
+  <si>
+    <t>Find dataset</t>
+  </si>
+  <si>
+    <t>weekly 10.11.</t>
+  </si>
+  <si>
+    <t>weekly 17.11.</t>
+  </si>
+  <si>
+    <t>weekly 1.12.</t>
+  </si>
+  <si>
+    <t>weekly 24.11.</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -37,7 +247,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -45,12 +255,95 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +623,206 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.44140625" style="6" customWidth="1"/>
+    <col min="5" max="5" width="20.33203125" style="6" customWidth="1"/>
+    <col min="6" max="12" width="8.88671875" style="6"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="13"/>
+      <c r="L1" s="13"/>
+    </row>
+    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="10"/>
+      <c r="D17" s="10"/>
+      <c r="E17" s="10"/>
+      <c r="F17" s="10"/>
+      <c r="G17" s="10"/>
+      <c r="H17" s="10"/>
+      <c r="I17" s="10"/>
+      <c r="J17" s="10"/>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+    </row>
+    <row r="18" spans="1:13" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+      <c r="F18" s="8"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="8"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="M19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update time management excel
</commit_message>
<xml_diff>
--- a/doc/time_management.xlsx
+++ b/doc/time_management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\antti\Documents\Courses\BDA\Bayes_project_2022\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D93B1D2-3C88-4387-8DD9-385716DADABC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDE7D3E7-C84B-4748-9EFE-DE82D51BC00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t xml:space="preserve"> </t>
   </si>
@@ -192,9 +192,6 @@
     <t>goal</t>
   </si>
   <si>
-    <t>Planning the project: Find data, project plan, project schedule</t>
-  </si>
-  <si>
     <t>Find dataset</t>
   </si>
   <si>
@@ -208,6 +205,68 @@
   </si>
   <si>
     <t>weekly 24.11.</t>
+  </si>
+  <si>
+    <t>Planning the project: Find data(done), project plan, project schedule</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Presentation 13.12. </t>
+  </si>
+  <si>
+    <t>Analysis, Report</t>
+  </si>
+  <si>
+    <t>Report, proof reading</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>49</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (4.-8.12.)</t>
+    </r>
+  </si>
+  <si>
+    <t>Peer grading</t>
+  </si>
+  <si>
+    <t>presentation, practise</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">50 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(12.-18.12.)</t>
+    </r>
+  </si>
+  <si>
+    <t>Project plan, project schedule(done)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Models i.e., Stan files, Decide the variables </t>
   </si>
 </sst>
 </file>
@@ -247,7 +306,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -304,11 +363,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -333,17 +412,27 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -624,65 +713,65 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomLeft" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="6" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" style="6" customWidth="1"/>
-    <col min="4" max="4" width="11.44140625" style="6" customWidth="1"/>
-    <col min="5" max="5" width="20.33203125" style="6" customWidth="1"/>
-    <col min="6" max="12" width="8.88671875" style="6"/>
+    <col min="1" max="1" width="19.28515625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="6" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" style="6" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="6" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" style="6" customWidth="1"/>
+    <col min="6" max="12" width="8.85546875" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="14" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="12" t="s">
+    <row r="1" spans="1:12" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-    </row>
-    <row r="2" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+    </row>
+    <row r="2" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4"/>
       <c r="B4" s="5"/>
       <c r="C4" s="5"/>
@@ -696,22 +785,25 @@
       <c r="K4" s="5"/>
       <c r="L4" s="5"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E5" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -725,22 +817,25 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -754,17 +849,20 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="E13" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -778,28 +876,20 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" s="11" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="E16" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="10"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="10"/>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-    </row>
-    <row r="18" spans="1:13" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7"/>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -813,12 +903,70 @@
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>10</v>
       </c>
       <c r="M19" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16"/>
+      <c r="I20" s="16"/>
+      <c r="J20" s="16"/>
+      <c r="K20" s="16"/>
+      <c r="L20" s="16"/>
+    </row>
+    <row r="21" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="13"/>
+      <c r="D21" s="13"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="13"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+    </row>
+    <row r="22" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>